<commit_message>
Update TEA for WFGD process
</commit_message>
<xml_diff>
--- a/TEA/TEA_WSS desulfurization.xlsx
+++ b/TEA/TEA_WSS desulfurization.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSID_17\Desktop\이혜정\3.2023\SCI 6. 환경팀\경제성 평가\WSS desulfurization process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSID_PC22\Documents\GitHub\TeamEnv\TEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82EAE0F-583D-484B-B656-2AEC74FA92EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11190" windowHeight="8940" activeTab="2"/>
+    <workbookView xWindow="20172" yWindow="0" windowWidth="20172" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Desulf" sheetId="5" r:id="rId1"/>
     <sheet name="Desulf EAC&amp;TPC" sheetId="6" r:id="rId2"/>
     <sheet name="Desulf revenue" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -467,7 +479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -786,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -794,9 +806,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -903,19 +912,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1">
@@ -956,7 +959,6 @@
     <xf numFmtId="176" fontId="7" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -976,9 +978,6 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1277,34 +1276,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.625" customWidth="1"/>
-    <col min="7" max="7" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="107.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="17.25" thickBot="1"/>
-    <row r="4" spans="2:11" ht="17.25" thickBot="1">
-      <c r="B4" s="5" t="s">
+    <row r="2" spans="2:10">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="18" thickBot="1"/>
+    <row r="4" spans="2:10" ht="18" thickBot="1">
+      <c r="B4" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1328,273 +1327,272 @@
       <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="61" t="s">
+      <c r="J4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="68">
+      <c r="C5" s="64">
         <v>147800</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="64">
         <v>461492</v>
       </c>
-      <c r="F5" s="69"/>
-      <c r="G5" s="68">
+      <c r="F5" s="65"/>
+      <c r="G5" s="64">
         <v>0.5</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="64">
         <v>1997</v>
       </c>
       <c r="I5" s="2">
         <f>C5*(F5/E5)^G5*(595.6/386.5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="7" t="s">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="68">
+      <c r="C6" s="64">
         <v>20000</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="64">
         <v>2500</v>
       </c>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70">
+      <c r="F6" s="65"/>
+      <c r="G6" s="66">
         <v>0.6</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="64">
         <v>1987</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f>C6*(F6/E6)^G6*(595.6/323.8)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="7" t="s">
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="68">
+      <c r="C7" s="64">
         <v>20000</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="64">
         <v>2500</v>
       </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70">
+      <c r="F7" s="65"/>
+      <c r="G7" s="66">
         <v>0.6</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="64">
         <v>1987</v>
       </c>
-      <c r="I7" s="65">
+      <c r="I7" s="61">
         <f>C7*(F7/E7)^G7*(595.6/323.8)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="7" t="s">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="64">
         <v>165000</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="D8" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="64">
         <v>359263</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="3">
+      <c r="F8" s="41"/>
+      <c r="G8">
         <v>0.6</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <v>1998</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f>C8*(F8/E8)^G8*(595.6/389.5)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="2:11" ht="17.25" thickBot="1">
-      <c r="B9" s="8" t="s">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="2:10" ht="18" thickBot="1">
+      <c r="B9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="64">
         <v>165000</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="64">
         <v>359263</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="3">
+      <c r="F9" s="41"/>
+      <c r="G9">
         <v>0.6</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <v>1998</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <f>C9*(F9/E9)^G9*(595.6/389.5)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="71"/>
-    </row>
-    <row r="10" spans="2:11" ht="17.25" thickBot="1">
-      <c r="B10" s="40" t="s">
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="2:10" ht="18" thickBot="1">
+      <c r="B10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="45">
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="42">
         <f>SUM(I5:I9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="2:10">
+      <c r="B15" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="17.25" thickBot="1"/>
-    <row r="17" spans="1:4" ht="17.25" thickBot="1">
-      <c r="B17" s="5" t="s">
+    <row r="16" spans="2:10" ht="18" thickBot="1"/>
+    <row r="17" spans="1:4" ht="18" thickBot="1">
+      <c r="B17" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="39">
+      <c r="C18" s="67"/>
+      <c r="D18" s="38">
         <f>C18*C31*C28</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="39">
+      <c r="C19" s="63"/>
+      <c r="D19" s="38">
         <f>C19*C31*C28</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="39">
+      <c r="C20" s="63"/>
+      <c r="D20" s="38">
         <f>C20*C31*C28</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="39">
+      <c r="C21" s="63"/>
+      <c r="D21" s="38">
         <f>C21*C30*C28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" thickBot="1">
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="1:4" ht="18" thickBot="1">
+      <c r="B22" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="39">
+      <c r="C22" s="68"/>
+      <c r="D22" s="38">
         <f>C22*C31*C28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" thickBot="1">
-      <c r="B23" s="40" t="s">
+    <row r="23" spans="1:4" ht="18" thickBot="1">
+      <c r="B23" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="62">
+      <c r="C23" s="40"/>
+      <c r="D23" s="58">
         <f>SUM(D18:D22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" thickBot="1"/>
-    <row r="28" spans="1:4" ht="17.25" thickBot="1">
-      <c r="B28" s="6" t="s">
+    <row r="27" spans="1:4" ht="18" thickBot="1"/>
+    <row r="28" spans="1:4" ht="18" thickBot="1">
+      <c r="B28" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C28" s="2">
         <f>8500*3600</f>
         <v>30600000</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>8500</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="64">
+      <c r="C29" s="60">
         <v>0.06</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="44">
         <v>-8.8900000000000003E-10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" thickBot="1">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:4" ht="18" thickBot="1">
+      <c r="A31" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="48">
+      <c r="C31" s="45">
         <v>7.9500000000000001E-9</v>
       </c>
     </row>
@@ -1605,604 +1603,604 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="2" max="2" width="55.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="17.25" thickBot="1">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:11" ht="18" thickBot="1">
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="I3" s="27" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="I3" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-    </row>
-    <row r="4" spans="2:11" ht="17.25" thickBot="1">
-      <c r="B4" s="12" t="s">
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+    </row>
+    <row r="4" spans="2:11" ht="18" thickBot="1">
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="I5" s="31" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="I5" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="51"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="48"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="20"/>
-      <c r="I6" s="17" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="19"/>
+      <c r="I6" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="49">
         <f>SUM(E29*0.01)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>30</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="43">
         <f>Desulf!I10</f>
         <v>0</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="52"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>10</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="19">
         <f>SUM(E29*0.1)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="K8" s="50" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>5</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <f>SUM(E29*0.05)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="63">
+      <c r="K9" s="59">
         <f>Desulf!D23</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>10</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <f>SUM(E29*0.1)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="34"/>
-      <c r="K10" s="54" t="s">
+      <c r="J10" s="33"/>
+      <c r="K10" s="51" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>5</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <f>SUM(E29*0.05)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="57" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="20"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="20"/>
-      <c r="I12" s="17" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="19"/>
+      <c r="I12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="36" t="s">
+      <c r="J12" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="55">
+      <c r="K12" s="52">
         <f>SUM(K6*0.04)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="20"/>
-      <c r="I13" s="17" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="19"/>
+      <c r="I13" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="52">
+      <c r="K13" s="49">
         <f>SUM(K25*0.15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>8</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="19">
         <f>SUM(E29*0.08)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="52">
+      <c r="K14" s="49">
         <f>SUM(K13*0.3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>2</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <f>SUM(E29*0.02)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="J15" s="34" t="s">
+      <c r="J15" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="52">
+      <c r="K15" s="49">
         <f>SUM(K12*0.15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>8</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <f>SUM(E29*0.08)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="K16" s="52">
+      <c r="K16" s="49">
         <f>SUM(K13*0.15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>2</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f>SUM(E29*0.02)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="52"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="49"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="20"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="20"/>
-      <c r="I18" s="22" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="19"/>
+      <c r="I18" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="34" t="s">
+      <c r="J18" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="K18" s="52">
+      <c r="K18" s="49">
         <f>SUM(0.6*K29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="20">
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="19">
         <f>SUM(E7:E17)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="52"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="49"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="20"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="20"/>
-      <c r="I20" s="22" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="19"/>
+      <c r="I20" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J20" s="34"/>
-      <c r="K20" s="52"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="49"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="20"/>
-      <c r="I21" s="17" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="19"/>
+      <c r="I21" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="K21" s="52">
+      <c r="K21" s="49">
         <f>SUM(K13*0.175)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>5</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="19">
         <f>SUM(E29*0.05)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="37" t="s">
+      <c r="I22" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="K22" s="52">
+      <c r="K22" s="49">
         <f>SUM(K25*0.11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="17">
         <v>5</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="19">
         <f>SUM(E29*0.05)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="37" t="s">
+      <c r="J23" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="52">
+      <c r="K23" s="49">
         <f>SUM(K25*0.035)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="17">
         <v>5</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="19">
         <f>SUM(E29*0.05)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="52"/>
-    </row>
-    <row r="25" spans="2:11" ht="17.25" thickBot="1">
-      <c r="B25" s="20" t="s">
+      <c r="I24" s="16"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="49"/>
+    </row>
+    <row r="25" spans="2:11" ht="18" thickBot="1">
+      <c r="B25" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="17">
         <v>5</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="19">
         <f>SUM(E29*0.05)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="I25" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J25" s="25"/>
-      <c r="K25" s="56">
+      <c r="J25" s="24"/>
+      <c r="K25" s="53">
         <f>SUM(K27/0.49425)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="20"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="20"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="57"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="54"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="20">
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="19">
         <f>SUM(E22:E25)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="57">
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="54">
         <f>SUM(K6:K12,K15,0.6*K12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="20"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="20"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="58"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="19"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="55"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="16">
         <v>100</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="17">
         <v>100</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="19">
         <f>SUM(E7*100/D7)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11" t="s">
+      <c r="I29" s="10"/>
+      <c r="J29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="K29" s="58">
+      <c r="K29" s="55">
         <f>(K12+K13+K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="16">
         <v>20</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="20">
         <v>20</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="19">
         <f>SUM(E29*0.2)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="59">
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="56">
         <f>SUM(K6:K23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="16">
         <v>20</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="20">
         <v>20</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="19">
         <f>SUM(E29*0.2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="20"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="20"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="16">
+      <c r="D33" s="22"/>
+      <c r="E33" s="15">
         <f>SUM(E29:E31)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B34" s="24" t="s">
+    <row r="34" spans="2:5" ht="18" thickBot="1">
+      <c r="B34" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="24">
+      <c r="D34" s="25"/>
+      <c r="E34" s="23">
         <f>SUM(E33/((1-(1/((1.05)^25)))/0.07))</f>
         <v>0</v>
       </c>
@@ -2214,42 +2212,42 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="3" max="3" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="18.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="17.25" thickBot="1"/>
-    <row r="2" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B2" s="5"/>
-      <c r="C2" s="75" t="s">
+    <row r="1" spans="2:5" ht="18" thickBot="1"/>
+    <row r="2" spans="2:5" ht="18" thickBot="1">
+      <c r="B2" s="4"/>
+      <c r="C2" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="40" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="2:5" ht="18" thickBot="1">
+      <c r="B3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="74">
+      <c r="C3" s="71"/>
+      <c r="D3" s="69">
         <v>500</v>
       </c>
-      <c r="E3" s="77">
+      <c r="E3" s="72">
         <f>C3*D3*8500</f>
         <v>0</v>
       </c>

</xml_diff>